<commit_message>
Actualizacion de Hoja de Ruta
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB067CDE-213F-45B8-8CEA-ED2DAC864B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D04E1D-9B99-4AAA-9C08-89758767F7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>Estado de completado</t>
   </si>
   <si>
-    <t>nada</t>
-  </si>
-  <si>
     <t>Desarollar todos los ABM y listado de entidades básicas</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>25/07/2025 - 01/08/2025</t>
+  </si>
+  <si>
+    <t>Voy a hacer el la lectura de la entidad menu</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +481,7 @@
     <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -506,7 +506,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -538,7 +538,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -546,17 +546,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,64 +564,64 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificacion clase Database para consultas escalares, y modificacion de clase Usuario para generar usuarios desde procedimiento almacenado en DB
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D04E1D-9B99-4AAA-9C08-89758767F7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028D2E78-9D9B-447D-A08B-29F247A33C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10050" yWindow="2745" windowWidth="16500" windowHeight="8055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hitos" sheetId="1" r:id="rId1"/>
+    <sheet name="Tareas divididas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Etapas</t>
   </si>
@@ -118,6 +119,24 @@
   </si>
   <si>
     <t>Voy a hacer el la lectura de la entidad menu</t>
+  </si>
+  <si>
+    <t>Leandro</t>
+  </si>
+  <si>
+    <t>Ezequiel</t>
+  </si>
+  <si>
+    <t>Franco</t>
+  </si>
+  <si>
+    <t>ABM de Productos, Categorias, Sub Categorias</t>
+  </si>
+  <si>
+    <t>ABM de Usuarios, Listado de mesas</t>
+  </si>
+  <si>
+    <t>Funcion de mesero</t>
   </si>
 </sst>
 </file>
@@ -471,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,4 +649,47 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A145C94-22D4-4EE2-B2BF-E734809676B4}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Avances en ABM de usuarios
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Prog III\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028D2E78-9D9B-447D-A08B-29F247A33C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2BB6ED-7B93-4179-A74A-C8FC4F19ED1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10050" yWindow="2745" windowWidth="16500" windowHeight="8055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hitos" sheetId="1" r:id="rId1"/>
     <sheet name="Tareas divididas" sheetId="2" r:id="rId2"/>
+    <sheet name="Usuarios" sheetId="4" r:id="rId3"/>
+    <sheet name="Niveles de Usuarios" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Etapas</t>
   </si>
@@ -137,6 +139,48 @@
   </si>
   <si>
     <t>Funcion de mesero</t>
+  </si>
+  <si>
+    <t>Numero Nivel</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Gerente</t>
+  </si>
+  <si>
+    <t>Mesero</t>
+  </si>
+  <si>
+    <t>Escalable, agregando más niveles</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Tipo Perfil</t>
+  </si>
+  <si>
+    <t>Admin123!</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Gerente123!</t>
+  </si>
+  <si>
+    <t>Mesero123!</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>idNivel</t>
   </si>
 </sst>
 </file>
@@ -185,7 +229,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -215,11 +289,43 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F1A5CD0A-F7E9-4B57-8AEF-6101F9482C08}" name="Etapas" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{96EA57F0-50F9-4EB2-8AAA-AD40893AC75C}" name="Fechas" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F1A5CD0A-F7E9-4B57-8AEF-6101F9482C08}" name="Etapas" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{96EA57F0-50F9-4EB2-8AAA-AD40893AC75C}" name="Fechas" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{F8C68D03-1E3C-456E-9908-D4B4678109B4}" name="Descripcion"/>
     <tableColumn id="4" xr3:uid="{5D1EFE42-C861-43ED-B78D-09D644B4EED7}" name="Comentarios"/>
     <tableColumn id="5" xr3:uid="{A9C06BD5-48AC-4E68-B0A4-55D8AFF9842C}" name="Estado de completado"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92A336DC-F41A-46B5-9826-9A31307311E6}" name="Tabla3" displayName="Tabla3" ref="A1:D4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:D4" xr:uid="{92A336DC-F41A-46B5-9826-9A31307311E6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{C800D0F1-4909-436B-AF33-A319483053DF}" name="Usuario" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8384088B-713A-417C-A564-473968BDF780}" name="Contraseña" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{32750CE2-D90D-4530-8AAE-77E423C5B9CA}" name="Tipo Perfil" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{35D8C34A-A2C6-4C8E-9641-C229A7BB9064}" name="idNivel" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C2CE8B9-BAA5-45FA-AE8E-49CFE6D72DA0}" name="Tabla1" displayName="Tabla1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+  <autoFilter ref="A1:B5" xr:uid="{3C2CE8B9-BAA5-45FA-AE8E-49CFE6D72DA0}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4528DBEB-2CAF-495F-A675-9429F6DC1241}" name="Numero Nivel" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C555297D-EE7B-4C41-B7B7-5ED276C43E39}" name="Nombre" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -490,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A145C94-22D4-4EE2-B2BF-E734809676B4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,4 +798,142 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA42346-F1E5-4673-9EC4-D5B07C8A8D64}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>123456</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>654321</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE512EC4-7609-401A-9D9A-FB8C9F31E43B}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Puesta en comun y division de tareas
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Prog III\tpi-prog-III-7B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2BB6ED-7B93-4179-A74A-C8FC4F19ED1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A84DC11-2C5D-4F1A-893D-525A5DC9FC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hitos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Etapas</t>
   </si>
@@ -132,15 +132,6 @@
     <t>Franco</t>
   </si>
   <si>
-    <t>ABM de Productos, Categorias, Sub Categorias</t>
-  </si>
-  <si>
-    <t>ABM de Usuarios, Listado de mesas</t>
-  </si>
-  <si>
-    <t>Funcion de mesero</t>
-  </si>
-  <si>
     <t>Numero Nivel</t>
   </si>
   <si>
@@ -181,6 +172,12 @@
   </si>
   <si>
     <t>idNivel</t>
+  </si>
+  <si>
+    <t>Stock, Bajas logicas de categorias y menus</t>
+  </si>
+  <si>
+    <t>Reportes, Armado procedimiento de suma del total a pagar, abm mesas</t>
   </si>
 </sst>
 </file>
@@ -300,7 +297,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92A336DC-F41A-46B5-9826-9A31307311E6}" name="Tabla3" displayName="Tabla3" ref="A1:D4" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{92A336DC-F41A-46B5-9826-9A31307311E6}" name="Tabla3" displayName="Tabla3" ref="A1:D4" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:D4" xr:uid="{92A336DC-F41A-46B5-9826-9A31307311E6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -308,24 +305,24 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C800D0F1-4909-436B-AF33-A319483053DF}" name="Usuario" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{8384088B-713A-417C-A564-473968BDF780}" name="Contraseña" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{32750CE2-D90D-4530-8AAE-77E423C5B9CA}" name="Tipo Perfil" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{35D8C34A-A2C6-4C8E-9641-C229A7BB9064}" name="idNivel" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{C800D0F1-4909-436B-AF33-A319483053DF}" name="Usuario" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{8384088B-713A-417C-A564-473968BDF780}" name="Contraseña" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{32750CE2-D90D-4530-8AAE-77E423C5B9CA}" name="Tipo Perfil" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{35D8C34A-A2C6-4C8E-9641-C229A7BB9064}" name="idNivel" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C2CE8B9-BAA5-45FA-AE8E-49CFE6D72DA0}" name="Tabla1" displayName="Tabla1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C2CE8B9-BAA5-45FA-AE8E-49CFE6D72DA0}" name="Tabla1" displayName="Tabla1" ref="A1:B5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B5" xr:uid="{3C2CE8B9-BAA5-45FA-AE8E-49CFE6D72DA0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4528DBEB-2CAF-495F-A675-9429F6DC1241}" name="Numero Nivel" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{C555297D-EE7B-4C41-B7B7-5ED276C43E39}" name="Nombre" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{4528DBEB-2CAF-495F-A675-9429F6DC1241}" name="Numero Nivel" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C555297D-EE7B-4C41-B7B7-5ED276C43E39}" name="Nombre" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -596,14 +593,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
@@ -759,40 +756,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A145C94-22D4-4EE2-B2BF-E734809676B4}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
+      <c r="B4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -817,27 +811,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -848,10 +842,10 @@
         <v>123456</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -862,10 +856,10 @@
         <v>654321</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -894,10 +888,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -905,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -913,7 +907,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -921,12 +915,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1"/>
     </row>

</xml_diff>

<commit_message>
Actualización de inserts y procedures
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A84DC11-2C5D-4F1A-893D-525A5DC9FC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378E01A7-289E-48D0-BD2F-EF42952BC5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hitos" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Etapas</t>
   </si>
@@ -174,10 +174,13 @@
     <t>idNivel</t>
   </si>
   <si>
-    <t>Stock, Bajas logicas de categorias y menus</t>
-  </si>
-  <si>
-    <t>Reportes, Armado procedimiento de suma del total a pagar, abm mesas</t>
+    <t>Reportes, Armado procedimiento de suma del total a pagar, abm mesas, asignar mesero a mesa, Validaciones</t>
+  </si>
+  <si>
+    <t>Gestion de ordenes y pedidos, filtros y búsquedas mesero, Validaciones</t>
+  </si>
+  <si>
+    <t>Stock, Bajas logicas de categorias y menus, filtros y búsquedas gerencia, Validaciones</t>
   </si>
 </sst>
 </file>
@@ -758,14 +761,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A145C94-22D4-4EE2-B2BF-E734809676B4}">
   <dimension ref="A2:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,20 +776,23 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -798,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA42346-F1E5-4673-9EC4-D5B07C8A8D64}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Avances administración de mesas + Fix de login + Procedures para gestion de mesas
</commit_message>
<xml_diff>
--- a/Hoja de ruta.xlsx
+++ b/Hoja de ruta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Salchy\UTN\Cursada 2025\[TRABAJOS PRACTICOS]\tpi-prog-III-7B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lcorrea\Desktop\Salchy\UTN\Prog III\tpi-prog-III-7B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378E01A7-289E-48D0-BD2F-EF42952BC5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F48FD4-B0FC-42B6-ABE6-92D08594E76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13935" yWindow="0" windowWidth="13935" windowHeight="16200" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hitos" sheetId="1" r:id="rId1"/>
@@ -596,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:C9"/>
     </sheetView>
   </sheetViews>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA42346-F1E5-4673-9EC4-D5B07C8A8D64}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>